<commit_message>
import clients - overwriting if exist
</commit_message>
<xml_diff>
--- a/public/uploaded-files/templates/import-clients.xlsx
+++ b/public/uploaded-files/templates/import-clients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\upwork\Firestore-PHP\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ousse\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB6507A-678C-4C54-86F5-97302A3F2BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{65272E62-0D7E-4BED-B810-557CB620DEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="1" r:id="rId1"/>
@@ -427,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -436,12 +436,11 @@
     <col min="1" max="1" width="15.69921875" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.69921875" style="4" customWidth="1"/>
     <col min="3" max="3" width="14.296875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.19921875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.796875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.09765625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11.19921875" style="4"/>
-    <col min="8" max="8" width="13.296875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="11.796875" style="4" customWidth="1"/>
+    <col min="4" max="5" width="14.19921875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.796875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.09765625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="11.19921875" style="4"/>
+    <col min="9" max="9" width="13.296875" style="4" customWidth="1"/>
     <col min="10" max="10" width="15.296875" style="4" customWidth="1"/>
     <col min="11" max="12" width="9.8984375" style="4" customWidth="1"/>
     <col min="13" max="13" width="11.19921875" style="4"/>
@@ -463,19 +462,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
import clients from CSV bug fixed
</commit_message>
<xml_diff>
--- a/public/uploaded-files/templates/import-clients.xlsx
+++ b/public/uploaded-files/templates/import-clients.xlsx
@@ -8,93 +8,115 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ousse\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65272E62-0D7E-4BED-B810-557CB620DEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{498E04C6-552C-4FCF-A17E-A702AF1A7BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>first_name_1</t>
-  </si>
-  <si>
-    <t>last_name_1</t>
-  </si>
-  <si>
-    <t>email_1</t>
-  </si>
-  <si>
-    <t>phone_1</t>
-  </si>
-  <si>
-    <t>first_name_2</t>
-  </si>
-  <si>
-    <t>last_name_2</t>
-  </si>
-  <si>
-    <t>email_2</t>
-  </si>
-  <si>
-    <t>phone_2</t>
-  </si>
-  <si>
-    <t>address_1</t>
-  </si>
-  <si>
-    <t>address_2</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>zip</t>
-  </si>
-  <si>
-    <t>home_type</t>
-  </si>
-  <si>
-    <t>notes</t>
+    <t>First name (Client's partner)</t>
+  </si>
+  <si>
+    <t>First name (Client)</t>
+  </si>
+  <si>
+    <t>Last name (Client)</t>
+  </si>
+  <si>
+    <t>Email address (Client)</t>
+  </si>
+  <si>
+    <t>Phone number (Client)</t>
+  </si>
+  <si>
+    <t>Last name (Client's partner)</t>
+  </si>
+  <si>
+    <t>Email address (Client's partner)</t>
+  </si>
+  <si>
+    <t>Phone number (Client's partner)</t>
+  </si>
+  <si>
+    <t>Address (line 1)</t>
+  </si>
+  <si>
+    <t>Address (line 2)</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Realtor notes</t>
+  </si>
+  <si>
+    <t>Home Type (Single, Townhome, Condo, Other)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <scheme val="major"/>
+      <color theme="0"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -102,25 +124,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,71 +467,73 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.69921875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.69921875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.296875" style="4" customWidth="1"/>
-    <col min="4" max="5" width="14.19921875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13.796875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.09765625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="11.19921875" style="4"/>
-    <col min="9" max="9" width="13.296875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="15.296875" style="4" customWidth="1"/>
-    <col min="11" max="12" width="9.8984375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="11.19921875" style="4"/>
-    <col min="14" max="14" width="13.5" style="5" customWidth="1"/>
-    <col min="15" max="15" width="11.19921875" style="5"/>
+    <col min="1" max="1" width="18.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.69921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.19921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.8984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.69921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.8984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.09765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="45.69921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.8984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.19921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" s="7" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>